<commit_message>
Añadiendo actualizacion al horario automatico
</commit_message>
<xml_diff>
--- a/Copia de Creación de Turnos y roles de la semana. CC097.xlsx
+++ b/Copia de Creación de Turnos y roles de la semana. CC097.xlsx
@@ -4,7 +4,6 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Empleados" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Horario" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="23">
   <si>
     <t>Empleados</t>
   </si>
@@ -41,8 +40,10 @@
     <t>Adrián Martos</t>
   </si>
   <si>
-    <t>10:00 - 14:00
-16:30 - 20:30</t>
+    <t>10:00-14:00 / 16:30-20:30</t>
+  </si>
+  <si>
+    <t>—</t>
   </si>
   <si>
     <t>Jose Peinado</t>
@@ -51,15 +52,15 @@
     <t>Javier Lopez</t>
   </si>
   <si>
-    <t>10:00 - 14:00</t>
+    <t>16:30-20:30</t>
+  </si>
+  <si>
+    <t>10:00-14:00</t>
   </si>
   <si>
     <t>Hilario Pastrana</t>
   </si>
   <si>
-    <t>16:30 - 20:30</t>
-  </si>
-  <si>
     <t>Fran Catena</t>
   </si>
   <si>
@@ -78,80 +79,14 @@
     <t>María Ruiz</t>
   </si>
   <si>
-    <t>9:00 - 14:00</t>
-  </si>
-  <si>
-    <t>9:00 - 13:00</t>
-  </si>
-  <si>
-    <t>Día</t>
-  </si>
-  <si>
-    <t>Turno Mañana</t>
-  </si>
-  <si>
-    <t>Turno Tarde</t>
-  </si>
-  <si>
-    <t>Turno Doble</t>
-  </si>
-  <si>
-    <t>Compras</t>
-  </si>
-  <si>
-    <t>Ventas</t>
-  </si>
-  <si>
-    <t>Adrián Martos, Fran Catena, Fran Cervilla, Jose Manuel, Cinthya Suazo</t>
-  </si>
-  <si>
-    <t>Javier Lopez, Hilario Pastrana, Antonio Ferron, María Ruiz</t>
-  </si>
-  <si>
-    <t>Adrián Martos, Jose Peinado, Hilario Pastrana, Fran Cervilla, Jose Manuel, Antonio Ferron, María Ruiz</t>
-  </si>
-  <si>
-    <t>Adrián Martos, Fran Catena, Javier Lopez, Hilario Pastrana</t>
-  </si>
-  <si>
-    <t>Fran Cervilla, Jose Manuel, Cinthya Suazo, Antonio Ferron, María Ruiz</t>
-  </si>
-  <si>
-    <t>Doble</t>
-  </si>
-  <si>
-    <t>Mañana</t>
-  </si>
-  <si>
-    <t>Jose Peinado, Fran Cervilla, Antonio Ferron, María Ruiz</t>
-  </si>
-  <si>
-    <t>Miércoles</t>
-  </si>
-  <si>
-    <t>Adrián Martos, Fran Catena, Jose Manuel, Cinthya Suazo</t>
-  </si>
-  <si>
-    <t>Jose Peinado, Javier Lopez, Fran Catena, Cinthya Suazo</t>
-  </si>
-  <si>
-    <t>Jose Manuel, Cinthya Suazo, Antonio Ferron, María Ruiz</t>
-  </si>
-  <si>
-    <t>Mañana / Doble</t>
-  </si>
-  <si>
-    <t>Jose Peinado, Javier Lopez, Hilario Pastrana, Fran Catena, Fran Cervilla, Jose Manuel</t>
-  </si>
-  <si>
-    <t>Adrián Martos, Jose Peinado</t>
+    <t>Sol Morales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -182,14 +117,8 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,12 +131,6 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -215,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -237,17 +160,8 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -258,10 +172,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -469,14 +379,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="38.38"/>
-    <col customWidth="1" min="2" max="2" width="26.13"/>
-    <col customWidth="1" min="3" max="3" width="21.38"/>
-    <col customWidth="1" min="4" max="4" width="23.0"/>
-    <col customWidth="1" min="5" max="5" width="22.38"/>
-    <col customWidth="1" min="6" max="6" width="25.75"/>
-    <col customWidth="1" min="7" max="7" width="34.75"/>
-    <col customWidth="1" min="8" max="8" width="36.5"/>
+    <col customWidth="1" min="1" max="1" width="16.0"/>
+    <col customWidth="1" min="2" max="7" width="25.0"/>
+    <col customWidth="1" min="8" max="8" width="6.63"/>
     <col hidden="1" min="9" max="9" width="12.63"/>
   </cols>
   <sheetData>
@@ -519,7 +424,9 @@
       <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
@@ -535,15 +442,17 @@
     </row>
     <row r="3" ht="51.0" customHeight="1">
       <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
@@ -562,25 +471,25 @@
     </row>
     <row r="4" ht="41.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H4" s="4">
         <v>32.0</v>
@@ -591,22 +500,22 @@
     </row>
     <row r="5" ht="45.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>9</v>
@@ -620,25 +529,25 @@
     </row>
     <row r="6" ht="47.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H6" s="4">
         <v>32.0</v>
@@ -649,7 +558,7 @@
     </row>
     <row r="7" ht="43.5" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
@@ -661,14 +570,16 @@
         <v>9</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="G7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="4">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
       <c r="I7" s="5">
         <v>32.0</v>
@@ -676,10 +587,10 @@
     </row>
     <row r="8" ht="58.5" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>14</v>
@@ -691,7 +602,7 @@
         <v>9</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>14</v>
@@ -705,25 +616,25 @@
     </row>
     <row r="9" ht="50.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H9" s="4">
         <v>32.0</v>
@@ -734,25 +645,25 @@
     </row>
     <row r="10" ht="47.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H10" s="4">
         <v>28.0</v>
@@ -763,224 +674,57 @@
     </row>
     <row r="11" ht="45.0" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="F11" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H11" s="6">
-        <v>24.0</v>
+        <v>20.0</v>
       </c>
       <c r="I11" s="5">
         <v>24.0</v>
       </c>
     </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="2" max="2" width="48.88"/>
-    <col customWidth="1" min="3" max="3" width="57.63"/>
-    <col customWidth="1" min="4" max="4" width="53.75"/>
-    <col customWidth="1" min="5" max="5" width="63.25"/>
-    <col customWidth="1" min="6" max="6" width="55.63"/>
-    <col customWidth="1" min="7" max="7" width="21.25"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="7"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>35</v>
+    <row r="12" ht="45.75" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="7">
+        <v>28.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>